<commit_message>
Added Entity and Sprite classes.
Methods should have proper syntax.

Signed-off-by: Eltee <rjlb.lt@gmail.com>
</commit_message>
<xml_diff>
--- a/Docs/B65_S1_Planification_Renaud_Bigras.xlsx
+++ b/Docs/B65_S1_Planification_Renaud_Bigras.xlsx
@@ -163,6 +163,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="K14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mr. Eltee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Les attributs de base d'Entity sont mis en place; classe abstraite.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C15" authorId="0">
       <text>
         <r>
@@ -184,6 +208,30 @@
           </rPr>
           <t xml:space="preserve">
 Coder les méthodes de déplacement, de collisions et les gets pour les attributs de base communs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K15" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mr. Eltee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Les méthodes sont mises en place; certaines méthodes sont en commentaires car les classes sont inexistantes encore.</t>
         </r>
       </text>
     </comment>
@@ -1780,706 +1828,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="172">
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
+  <dxfs count="211">
     <dxf>
       <font>
         <color rgb="FF255B01"/>
@@ -4408,6 +3757,1404 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -5117,7 +5864,6 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
       </c:pie3DChart>
     </c:plotArea>
     <c:legend>
@@ -5138,7 +5884,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5283,12 +6029,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="53250304"/>
-        <c:axId val="53272576"/>
+        <c:axId val="89503616"/>
+        <c:axId val="89505152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53250304"/>
+        <c:axId val="89503616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5304,14 +6049,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53272576"/>
+        <c:crossAx val="89505152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53272576"/>
+        <c:axId val="89505152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5347,7 +6092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53250304"/>
+        <c:crossAx val="89503616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5370,7 +6115,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5442,56 +6187,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:AA50" totalsRowCount="1" headerRowDxfId="171" dataDxfId="170" totalsRowDxfId="169">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:AA50" totalsRowCount="1" headerRowDxfId="210" dataDxfId="209" totalsRowDxfId="208">
   <tableColumns count="26">
-    <tableColumn id="1" name="Numéro de tâche" dataDxfId="168" totalsRowDxfId="142"/>
-    <tableColumn id="2" name="Description générale de la tâche" totalsRowFunction="count" dataDxfId="167" totalsRowDxfId="141"/>
-    <tableColumn id="3" name="Prédécesseurs" dataDxfId="166" totalsRowDxfId="140"/>
-    <tableColumn id="4" name="Niveau de priorité" dataDxfId="165" totalsRowDxfId="139"/>
-    <tableColumn id="5" name="Niveau de difficulté" dataDxfId="164" totalsRowDxfId="138"/>
-    <tableColumn id="6" name="Temps requis (minutes)" totalsRowFunction="sum" dataDxfId="163" totalsRowDxfId="137"/>
-    <tableColumn id="7" name="Prévision du Sprint où la tâche doit être terminée" dataDxfId="162" totalsRowDxfId="136"/>
-    <tableColumn id="8" name="Temps investis (minutes)" totalsRowFunction="sum" dataDxfId="161" totalsRowDxfId="135"/>
-    <tableColumn id="9" name="% d'avancement au Sprint 1" dataDxfId="160" totalsRowDxfId="134"/>
-    <tableColumn id="10" name="% d'avancement au Sprint 2" dataDxfId="159" totalsRowDxfId="133"/>
-    <tableColumn id="11" name="% d'avancement au Sprint 3" dataDxfId="158" totalsRowDxfId="132"/>
-    <tableColumn id="12" name="% d'avancement au Sprint 4" dataDxfId="157" totalsRowDxfId="131"/>
-    <tableColumn id="13" name="Pourquoi le retard" dataDxfId="156" totalsRowDxfId="130"/>
-    <tableColumn id="14" name="Moyens envisagés pour solutionner le problème" dataDxfId="155" totalsRowDxfId="129"/>
-    <tableColumn id="15" name="Sprint 1" dataDxfId="154" totalsRowDxfId="128">
+    <tableColumn id="1" name="Numéro de tâche" dataDxfId="207" totalsRowDxfId="103"/>
+    <tableColumn id="2" name="Description générale de la tâche" totalsRowFunction="count" dataDxfId="206" totalsRowDxfId="102"/>
+    <tableColumn id="3" name="Prédécesseurs" dataDxfId="205" totalsRowDxfId="101"/>
+    <tableColumn id="4" name="Niveau de priorité" dataDxfId="204" totalsRowDxfId="100"/>
+    <tableColumn id="5" name="Niveau de difficulté" dataDxfId="203" totalsRowDxfId="99"/>
+    <tableColumn id="6" name="Temps requis (minutes)" totalsRowFunction="sum" dataDxfId="202" totalsRowDxfId="98"/>
+    <tableColumn id="7" name="Prévision du Sprint où la tâche doit être terminée" dataDxfId="201" totalsRowDxfId="97"/>
+    <tableColumn id="8" name="Temps investis (minutes)" totalsRowFunction="sum" dataDxfId="200" totalsRowDxfId="96"/>
+    <tableColumn id="9" name="% d'avancement au Sprint 1" dataDxfId="199" totalsRowDxfId="95"/>
+    <tableColumn id="10" name="% d'avancement au Sprint 2" dataDxfId="198" totalsRowDxfId="94"/>
+    <tableColumn id="11" name="% d'avancement au Sprint 3" dataDxfId="197" totalsRowDxfId="93"/>
+    <tableColumn id="12" name="% d'avancement au Sprint 4" dataDxfId="196" totalsRowDxfId="92"/>
+    <tableColumn id="13" name="Pourquoi le retard" dataDxfId="195" totalsRowDxfId="91"/>
+    <tableColumn id="14" name="Moyens envisagés pour solutionner le problème" dataDxfId="194" totalsRowDxfId="90"/>
+    <tableColumn id="15" name="Sprint 1" dataDxfId="193" totalsRowDxfId="89">
       <calculatedColumnFormula>IF(OR($H13="",J13=""),"Indef",IF(J13&gt;=1,"Terminé",IF($H13&lt;=P$12,"Retard",IF(J13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Sprint 2" dataDxfId="153" totalsRowDxfId="127">
+    <tableColumn id="16" name="Sprint 2" dataDxfId="192" totalsRowDxfId="88">
       <calculatedColumnFormula>IF(OR($H13="",K13=""),"Indef",IF(K13&gt;=1,"Terminé",IF($H13&lt;=Q$12,"Retard",IF(K13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Sprint 3" dataDxfId="152" totalsRowDxfId="126">
+    <tableColumn id="17" name="Sprint 3" dataDxfId="191" totalsRowDxfId="87">
       <calculatedColumnFormula>IF(OR($H13="",L13=""),"Indef",IF(L13&gt;=1,"Terminé",IF($H13&lt;=R$12,"Retard",IF(L13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Sprint 4" dataDxfId="151" totalsRowDxfId="125">
+    <tableColumn id="18" name="Sprint 4" dataDxfId="190" totalsRowDxfId="86">
       <calculatedColumnFormula>IF(OR($H13="",M13=""),"Indef",IF(M13&gt;=1,"Terminé",IF($H13&lt;=S$12,"Retard",IF(M13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Prev 00" dataDxfId="150" totalsRowDxfId="124">
+    <tableColumn id="25" name="Prev 00" dataDxfId="189" totalsRowDxfId="85">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Prev 01" dataDxfId="149" totalsRowDxfId="123">
+    <tableColumn id="26" name="Prev 01" dataDxfId="188" totalsRowDxfId="84">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Prev 02" dataDxfId="148" totalsRowDxfId="122">
+    <tableColumn id="27" name="Prev 02" dataDxfId="187" totalsRowDxfId="83">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Prev 03" dataDxfId="147" totalsRowDxfId="121">
+    <tableColumn id="28" name="Prev 03" dataDxfId="186" totalsRowDxfId="82">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 4",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Temps S1" dataDxfId="146" totalsRowDxfId="120">
+    <tableColumn id="21" name="Temps S1" dataDxfId="185" totalsRowDxfId="81">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Temps S2" dataDxfId="145" totalsRowDxfId="119">
+    <tableColumn id="23" name="Temps S2" dataDxfId="184" totalsRowDxfId="80">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Temps S3" dataDxfId="144" totalsRowDxfId="118">
+    <tableColumn id="22" name="Temps S3" dataDxfId="183" totalsRowDxfId="79">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Temps S4" dataDxfId="143" totalsRowDxfId="117">
+    <tableColumn id="24" name="Temps S4" dataDxfId="182" totalsRowDxfId="78">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 4",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5787,7 +6532,7 @@
   <dimension ref="A1:AH195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="11.25"/>
@@ -6093,7 +6838,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L14" s="33">
         <v>0</v>
@@ -6189,7 +6934,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="33">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="L15" s="33">
         <v>0</v>
@@ -6283,7 +7028,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L16" s="33">
         <v>0</v>
@@ -11280,150 +12025,150 @@
     <mergeCell ref="C3:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:F26">
-    <cfRule type="cellIs" dxfId="77" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="49" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="50" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:M26">
-    <cfRule type="expression" dxfId="74" priority="36">
+    <cfRule type="expression" dxfId="74" priority="39">
       <formula>P13="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="37">
+    <cfRule type="expression" dxfId="73" priority="40">
       <formula>P13="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="38">
+    <cfRule type="expression" dxfId="72" priority="41">
       <formula>P13="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:F28">
-    <cfRule type="cellIs" dxfId="71" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="37" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="38" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:M28">
-    <cfRule type="expression" dxfId="68" priority="30">
+    <cfRule type="expression" dxfId="68" priority="33">
       <formula>P28="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="31">
+    <cfRule type="expression" dxfId="67" priority="34">
       <formula>P28="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="32">
+    <cfRule type="expression" dxfId="66" priority="35">
       <formula>P28="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:F43">
-    <cfRule type="cellIs" dxfId="65" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="31" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="32" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:M43">
-    <cfRule type="expression" dxfId="62" priority="24">
+    <cfRule type="expression" dxfId="62" priority="27">
       <formula>P29="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="25">
+    <cfRule type="expression" dxfId="61" priority="28">
       <formula>P29="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="26">
+    <cfRule type="expression" dxfId="60" priority="29">
       <formula>P29="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:F46">
-    <cfRule type="cellIs" dxfId="59" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="25" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="26" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:M46">
-    <cfRule type="expression" dxfId="56" priority="18">
+    <cfRule type="expression" dxfId="56" priority="21">
       <formula>P44="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="19">
+    <cfRule type="expression" dxfId="55" priority="22">
       <formula>P44="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="20">
+    <cfRule type="expression" dxfId="54" priority="23">
       <formula>P44="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:F27">
-    <cfRule type="cellIs" dxfId="53" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="20" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:M27">
-    <cfRule type="expression" dxfId="50" priority="12">
+    <cfRule type="expression" dxfId="50" priority="15">
       <formula>P27="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="13">
+    <cfRule type="expression" dxfId="49" priority="16">
       <formula>P27="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="14">
+    <cfRule type="expression" dxfId="48" priority="17">
       <formula>P27="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47:M47">
-    <cfRule type="expression" dxfId="47" priority="9">
+    <cfRule type="expression" dxfId="47" priority="12">
       <formula>P47="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="10">
+    <cfRule type="expression" dxfId="46" priority="13">
       <formula>P47="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="11">
+    <cfRule type="expression" dxfId="45" priority="14">
       <formula>P47="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:M48">
-    <cfRule type="expression" dxfId="44" priority="6">
+    <cfRule type="expression" dxfId="44" priority="9">
       <formula>P48="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="7">
+    <cfRule type="expression" dxfId="43" priority="10">
       <formula>P48="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="8">
+    <cfRule type="expression" dxfId="42" priority="11">
       <formula>P48="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:M49">
-    <cfRule type="expression" dxfId="41" priority="3">
+    <cfRule type="expression" dxfId="41" priority="6">
       <formula>P49="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="4">
+    <cfRule type="expression" dxfId="40" priority="7">
       <formula>P49="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="5">
+    <cfRule type="expression" dxfId="39" priority="8">
       <formula>P49="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -11433,12 +12178,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Serializer, Tileset and SpriteStore.
Made basic changes to Entity and Sprite to take SpriteStore into account.

Signed-off-by: Eltee <rjlb.lt@gmail.com>
</commit_message>
<xml_diff>
--- a/Docs/B65_S1_Planification_Renaud_Bigras.xlsx
+++ b/Docs/B65_S1_Planification_Renaud_Bigras.xlsx
@@ -259,6 +259,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="K17" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mr. Eltee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mis en place, manque seulement les algos pour donner accès a un spriteset et non pas une seule sprite par entité..</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C18" authorId="0">
       <text>
         <r>
@@ -304,6 +328,30 @@
           </rPr>
           <t xml:space="preserve">
 Mise en place d'un algo pour sauvegarder les objets Tileset en fichiers encryptés et d'un algo pour les charger au démarrage.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K19" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mr. Eltee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ajout de la classe Serializer qui ne sera pas utiliser dans le jeu en tant que tel, mais qui contient un main() servant à sauvegarder des objets serialisés.</t>
         </r>
       </text>
     </comment>
@@ -1462,7 +1510,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1639,12 +1687,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1792,26 +1851,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1823,12 +1862,567 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="211">
+  <dxfs count="175">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="#&quot; min&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="#&quot; min&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#&quot; tâches&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF255B01"/>
@@ -2143,21 +2737,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF255B01"/>
       </font>
       <fill>
@@ -2608,240 +3187,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF00A400"/>
       </font>
     </dxf>
@@ -2854,909 +3199,6 @@
       <font>
         <color rgb="FFA40000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#&quot; min&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#&quot; min&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#&quot; tâches&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5884,7 +5326,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6029,11 +5471,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="89503616"/>
-        <c:axId val="89505152"/>
+        <c:axId val="80139008"/>
+        <c:axId val="80140544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89503616"/>
+        <c:axId val="80139008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6049,14 +5491,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89505152"/>
+        <c:crossAx val="80140544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89505152"/>
+        <c:axId val="80140544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6092,7 +5534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89503616"/>
+        <c:crossAx val="80139008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6115,7 +5557,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6187,56 +5629,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:AA50" totalsRowCount="1" headerRowDxfId="210" dataDxfId="209" totalsRowDxfId="208">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:AA50" totalsRowCount="1" headerRowDxfId="174" dataDxfId="173" totalsRowDxfId="172">
   <tableColumns count="26">
-    <tableColumn id="1" name="Numéro de tâche" dataDxfId="207" totalsRowDxfId="103"/>
-    <tableColumn id="2" name="Description générale de la tâche" totalsRowFunction="count" dataDxfId="206" totalsRowDxfId="102"/>
-    <tableColumn id="3" name="Prédécesseurs" dataDxfId="205" totalsRowDxfId="101"/>
-    <tableColumn id="4" name="Niveau de priorité" dataDxfId="204" totalsRowDxfId="100"/>
-    <tableColumn id="5" name="Niveau de difficulté" dataDxfId="203" totalsRowDxfId="99"/>
-    <tableColumn id="6" name="Temps requis (minutes)" totalsRowFunction="sum" dataDxfId="202" totalsRowDxfId="98"/>
-    <tableColumn id="7" name="Prévision du Sprint où la tâche doit être terminée" dataDxfId="201" totalsRowDxfId="97"/>
-    <tableColumn id="8" name="Temps investis (minutes)" totalsRowFunction="sum" dataDxfId="200" totalsRowDxfId="96"/>
-    <tableColumn id="9" name="% d'avancement au Sprint 1" dataDxfId="199" totalsRowDxfId="95"/>
-    <tableColumn id="10" name="% d'avancement au Sprint 2" dataDxfId="198" totalsRowDxfId="94"/>
-    <tableColumn id="11" name="% d'avancement au Sprint 3" dataDxfId="197" totalsRowDxfId="93"/>
-    <tableColumn id="12" name="% d'avancement au Sprint 4" dataDxfId="196" totalsRowDxfId="92"/>
-    <tableColumn id="13" name="Pourquoi le retard" dataDxfId="195" totalsRowDxfId="91"/>
-    <tableColumn id="14" name="Moyens envisagés pour solutionner le problème" dataDxfId="194" totalsRowDxfId="90"/>
-    <tableColumn id="15" name="Sprint 1" dataDxfId="193" totalsRowDxfId="89">
+    <tableColumn id="1" name="Numéro de tâche" dataDxfId="171" totalsRowDxfId="25"/>
+    <tableColumn id="2" name="Description générale de la tâche" totalsRowFunction="count" dataDxfId="170" totalsRowDxfId="24"/>
+    <tableColumn id="3" name="Prédécesseurs" dataDxfId="169" totalsRowDxfId="23"/>
+    <tableColumn id="4" name="Niveau de priorité" dataDxfId="168" totalsRowDxfId="22"/>
+    <tableColumn id="5" name="Niveau de difficulté" dataDxfId="167" totalsRowDxfId="21"/>
+    <tableColumn id="6" name="Temps requis (minutes)" totalsRowFunction="sum" dataDxfId="166" totalsRowDxfId="20"/>
+    <tableColumn id="7" name="Prévision du Sprint où la tâche doit être terminée" dataDxfId="165" totalsRowDxfId="19"/>
+    <tableColumn id="8" name="Temps investis (minutes)" totalsRowFunction="sum" dataDxfId="164" totalsRowDxfId="18"/>
+    <tableColumn id="9" name="% d'avancement au Sprint 1" dataDxfId="163" totalsRowDxfId="17"/>
+    <tableColumn id="10" name="% d'avancement au Sprint 2" dataDxfId="162" totalsRowDxfId="16"/>
+    <tableColumn id="11" name="% d'avancement au Sprint 3" dataDxfId="161" totalsRowDxfId="15"/>
+    <tableColumn id="12" name="% d'avancement au Sprint 4" dataDxfId="160" totalsRowDxfId="14"/>
+    <tableColumn id="13" name="Pourquoi le retard" dataDxfId="159" totalsRowDxfId="13"/>
+    <tableColumn id="14" name="Moyens envisagés pour solutionner le problème" dataDxfId="158" totalsRowDxfId="12"/>
+    <tableColumn id="15" name="Sprint 1" dataDxfId="157" totalsRowDxfId="11">
       <calculatedColumnFormula>IF(OR($H13="",J13=""),"Indef",IF(J13&gt;=1,"Terminé",IF($H13&lt;=P$12,"Retard",IF(J13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Sprint 2" dataDxfId="192" totalsRowDxfId="88">
+    <tableColumn id="16" name="Sprint 2" dataDxfId="156" totalsRowDxfId="10">
       <calculatedColumnFormula>IF(OR($H13="",K13=""),"Indef",IF(K13&gt;=1,"Terminé",IF($H13&lt;=Q$12,"Retard",IF(K13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Sprint 3" dataDxfId="191" totalsRowDxfId="87">
+    <tableColumn id="17" name="Sprint 3" dataDxfId="155" totalsRowDxfId="9">
       <calculatedColumnFormula>IF(OR($H13="",L13=""),"Indef",IF(L13&gt;=1,"Terminé",IF($H13&lt;=R$12,"Retard",IF(L13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Sprint 4" dataDxfId="190" totalsRowDxfId="86">
+    <tableColumn id="18" name="Sprint 4" dataDxfId="154" totalsRowDxfId="8">
       <calculatedColumnFormula>IF(OR($H13="",M13=""),"Indef",IF(M13&gt;=1,"Terminé",IF($H13&lt;=S$12,"Retard",IF(M13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Prev 00" dataDxfId="189" totalsRowDxfId="85">
+    <tableColumn id="25" name="Prev 00" dataDxfId="153" totalsRowDxfId="7">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Prev 01" dataDxfId="188" totalsRowDxfId="84">
+    <tableColumn id="26" name="Prev 01" dataDxfId="152" totalsRowDxfId="6">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Prev 02" dataDxfId="187" totalsRowDxfId="83">
+    <tableColumn id="27" name="Prev 02" dataDxfId="151" totalsRowDxfId="5">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Prev 03" dataDxfId="186" totalsRowDxfId="82">
+    <tableColumn id="28" name="Prev 03" dataDxfId="150" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 4",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Temps S1" dataDxfId="185" totalsRowDxfId="81">
+    <tableColumn id="21" name="Temps S1" dataDxfId="149" totalsRowDxfId="3">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Temps S2" dataDxfId="184" totalsRowDxfId="80">
+    <tableColumn id="23" name="Temps S2" dataDxfId="148" totalsRowDxfId="2">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Temps S3" dataDxfId="183" totalsRowDxfId="79">
+    <tableColumn id="22" name="Temps S3" dataDxfId="147" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Temps S4" dataDxfId="182" totalsRowDxfId="78">
+    <tableColumn id="24" name="Temps S4" dataDxfId="146" totalsRowDxfId="0">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 4",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6532,7 +5974,7 @@
   <dimension ref="A1:AH195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="11.25"/>
@@ -6558,22 +6000,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="19.5" thickBot="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
       <c r="O1" s="40" t="s">
         <v>13</v>
       </c>
@@ -6589,7 +6031,7 @@
     </row>
     <row r="3" spans="1:34" ht="12" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="44" t="s">
         <v>72</v>
       </c>
       <c r="O3" s="28" t="s">
@@ -6598,37 +6040,37 @@
     </row>
     <row r="4" spans="1:34" ht="12" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="C4" s="50"/>
+      <c r="C4" s="45"/>
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:34" ht="12" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="C5" s="50"/>
+      <c r="C5" s="45"/>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:34" ht="12" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="C6" s="50"/>
+      <c r="C6" s="45"/>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:34" ht="12" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="C7" s="50"/>
+      <c r="C7" s="45"/>
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:34" ht="12" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="C8" s="50"/>
+      <c r="C8" s="45"/>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:34" ht="12" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="C9" s="50"/>
+      <c r="C9" s="45"/>
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:34" ht="12" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="45"/>
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:34">
@@ -7124,7 +6566,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="33">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="L17" s="33">
         <v>0</v>
@@ -7220,7 +6662,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="33">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="L18" s="33">
         <v>0</v>
@@ -7308,10 +6750,18 @@
       </c>
       <c r="H19" s="31"/>
       <c r="I19" s="29"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
+      <c r="J19" s="51">
+        <v>0</v>
+      </c>
+      <c r="K19" s="51">
+        <v>0.8</v>
+      </c>
+      <c r="L19" s="51">
+        <v>0</v>
+      </c>
+      <c r="M19" s="51">
+        <v>0</v>
+      </c>
       <c r="N19" s="34"/>
       <c r="O19" s="35"/>
       <c r="P19" s="8" t="str">
@@ -10039,24 +9489,24 @@
         <f>SUBTOTAL(109,[Temps investis (minutes)])</f>
         <v>25</v>
       </c>
-      <c r="J50" s="43"/>
-      <c r="K50" s="44"/>
-      <c r="L50" s="44"/>
-      <c r="M50" s="44"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="47"/>
       <c r="N50" s="34"/>
       <c r="O50" s="39"/>
-      <c r="P50" s="45"/>
-      <c r="Q50" s="45"/>
-      <c r="R50" s="45"/>
-      <c r="S50" s="45"/>
-      <c r="T50" s="45"/>
-      <c r="U50" s="45"/>
-      <c r="V50" s="45"/>
-      <c r="W50" s="45"/>
-      <c r="X50" s="45"/>
-      <c r="Y50" s="46"/>
-      <c r="Z50" s="45"/>
-      <c r="AA50" s="47"/>
+      <c r="P50" s="48"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="48"/>
+      <c r="S50" s="48"/>
+      <c r="T50" s="48"/>
+      <c r="U50" s="48"/>
+      <c r="V50" s="48"/>
+      <c r="W50" s="48"/>
+      <c r="X50" s="48"/>
+      <c r="Y50" s="49"/>
+      <c r="Z50" s="48"/>
+      <c r="AA50" s="50"/>
     </row>
     <row r="51" spans="2:27">
       <c r="B51" s="27"/>
@@ -12025,150 +11475,150 @@
     <mergeCell ref="C3:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:F26">
-    <cfRule type="cellIs" dxfId="77" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="51" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="52" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="53" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:M26">
-    <cfRule type="expression" dxfId="74" priority="39">
+    <cfRule type="expression" dxfId="103" priority="42">
       <formula>P13="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="40">
+    <cfRule type="expression" dxfId="102" priority="43">
       <formula>P13="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="41">
+    <cfRule type="expression" dxfId="101" priority="44">
       <formula>P13="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:F28">
-    <cfRule type="cellIs" dxfId="71" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="40" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="41" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:M28">
-    <cfRule type="expression" dxfId="68" priority="33">
+    <cfRule type="expression" dxfId="97" priority="36">
       <formula>P28="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="34">
+    <cfRule type="expression" dxfId="96" priority="37">
       <formula>P28="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="35">
+    <cfRule type="expression" dxfId="95" priority="38">
       <formula>P28="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:F43">
-    <cfRule type="cellIs" dxfId="65" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="34" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="35" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:M43">
-    <cfRule type="expression" dxfId="62" priority="27">
+    <cfRule type="expression" dxfId="91" priority="30">
       <formula>P29="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="28">
+    <cfRule type="expression" dxfId="90" priority="31">
       <formula>P29="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="29">
+    <cfRule type="expression" dxfId="89" priority="32">
       <formula>P29="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:F46">
-    <cfRule type="cellIs" dxfId="59" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="29" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:M46">
-    <cfRule type="expression" dxfId="56" priority="21">
+    <cfRule type="expression" dxfId="85" priority="24">
       <formula>P44="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="22">
+    <cfRule type="expression" dxfId="84" priority="25">
       <formula>P44="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="23">
+    <cfRule type="expression" dxfId="83" priority="26">
       <formula>P44="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:F27">
-    <cfRule type="cellIs" dxfId="53" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="22" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="23" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:M27">
-    <cfRule type="expression" dxfId="50" priority="15">
+    <cfRule type="expression" dxfId="79" priority="18">
       <formula>P27="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="16">
+    <cfRule type="expression" dxfId="78" priority="19">
       <formula>P27="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="17">
+    <cfRule type="expression" dxfId="77" priority="20">
       <formula>P27="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47:M47">
-    <cfRule type="expression" dxfId="47" priority="12">
+    <cfRule type="expression" dxfId="76" priority="15">
       <formula>P47="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="13">
+    <cfRule type="expression" dxfId="75" priority="16">
       <formula>P47="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="14">
+    <cfRule type="expression" dxfId="74" priority="17">
       <formula>P47="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:M48">
-    <cfRule type="expression" dxfId="44" priority="9">
+    <cfRule type="expression" dxfId="73" priority="12">
       <formula>P48="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="10">
+    <cfRule type="expression" dxfId="72" priority="13">
       <formula>P48="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="11">
+    <cfRule type="expression" dxfId="71" priority="14">
       <formula>P48="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:M49">
-    <cfRule type="expression" dxfId="41" priority="6">
+    <cfRule type="expression" dxfId="70" priority="9">
       <formula>P49="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="7">
+    <cfRule type="expression" dxfId="69" priority="10">
       <formula>P49="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="8">
+    <cfRule type="expression" dxfId="68" priority="11">
       <formula>P49="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -12178,7 +11628,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -12188,7 +11638,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -12198,6 +11648,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12207,13 +11687,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
+  <conditionalFormatting sqref="K19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Loading of tilesets as tile names and URL references implemented. Time wasted...
Signed-off-by: Eltee <rjlb.lt@gmail.com>
</commit_message>
<xml_diff>
--- a/Docs/B65_S1_Planification_Renaud_Bigras.xlsx
+++ b/Docs/B65_S1_Planification_Renaud_Bigras.xlsx
@@ -351,7 +351,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Ajout de la classe Serializer qui ne sera pas utiliser dans le jeu en tant que tel, mais qui contient un main() servant à sauvegarder des objets serialisés.</t>
+Doit mettre en place une méthode de lire un dossier contenant des tilesets contenus dans un dossier.
+-EDIT: Le jeu charge les tilesets en tant que noms de tuiles et references URL aux fichiers lors du début du jeu.</t>
         </r>
       </text>
     </comment>
@@ -1106,7 +1107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
   <si>
     <t>Numéro de tâche</t>
   </si>
@@ -1851,17 +1852,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="distributed" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1886,12 +1876,23 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="distributed" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="175">
+  <dxfs count="94">
     <dxf>
       <font>
         <b val="0"/>
@@ -2425,81 +2426,594 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF255B01"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF5B0101"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF01125B"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color rgb="FF05015B"/>
+          <color auto="1"/>
         </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <top/>
+        <bottom/>
       </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="1"/>
     </dxf>
     <dxf>
       <font>
@@ -3200,1995 +3714,6 @@
         <color rgb="FFA40000"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="1"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5294,7 +3819,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
@@ -5326,7 +3851,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5403,7 +3928,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>320</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>505</c:v>
@@ -5459,7 +3984,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -5471,11 +3996,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="80139008"/>
-        <c:axId val="80140544"/>
+        <c:axId val="96957952"/>
+        <c:axId val="96959488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80139008"/>
+        <c:axId val="96957952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5491,14 +4016,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80140544"/>
+        <c:crossAx val="96959488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80140544"/>
+        <c:axId val="96959488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5534,7 +4059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80139008"/>
+        <c:crossAx val="96957952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5557,7 +4082,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5629,56 +4154,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:AA50" totalsRowCount="1" headerRowDxfId="174" dataDxfId="173" totalsRowDxfId="172">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:AA50" totalsRowCount="1" headerRowDxfId="54" dataDxfId="53" totalsRowDxfId="52">
   <tableColumns count="26">
-    <tableColumn id="1" name="Numéro de tâche" dataDxfId="171" totalsRowDxfId="25"/>
-    <tableColumn id="2" name="Description générale de la tâche" totalsRowFunction="count" dataDxfId="170" totalsRowDxfId="24"/>
-    <tableColumn id="3" name="Prédécesseurs" dataDxfId="169" totalsRowDxfId="23"/>
-    <tableColumn id="4" name="Niveau de priorité" dataDxfId="168" totalsRowDxfId="22"/>
-    <tableColumn id="5" name="Niveau de difficulté" dataDxfId="167" totalsRowDxfId="21"/>
-    <tableColumn id="6" name="Temps requis (minutes)" totalsRowFunction="sum" dataDxfId="166" totalsRowDxfId="20"/>
-    <tableColumn id="7" name="Prévision du Sprint où la tâche doit être terminée" dataDxfId="165" totalsRowDxfId="19"/>
-    <tableColumn id="8" name="Temps investis (minutes)" totalsRowFunction="sum" dataDxfId="164" totalsRowDxfId="18"/>
-    <tableColumn id="9" name="% d'avancement au Sprint 1" dataDxfId="163" totalsRowDxfId="17"/>
-    <tableColumn id="10" name="% d'avancement au Sprint 2" dataDxfId="162" totalsRowDxfId="16"/>
-    <tableColumn id="11" name="% d'avancement au Sprint 3" dataDxfId="161" totalsRowDxfId="15"/>
-    <tableColumn id="12" name="% d'avancement au Sprint 4" dataDxfId="160" totalsRowDxfId="14"/>
-    <tableColumn id="13" name="Pourquoi le retard" dataDxfId="159" totalsRowDxfId="13"/>
-    <tableColumn id="14" name="Moyens envisagés pour solutionner le problème" dataDxfId="158" totalsRowDxfId="12"/>
-    <tableColumn id="15" name="Sprint 1" dataDxfId="157" totalsRowDxfId="11">
+    <tableColumn id="1" name="Numéro de tâche" dataDxfId="51" totalsRowDxfId="25"/>
+    <tableColumn id="2" name="Description générale de la tâche" totalsRowFunction="count" dataDxfId="50" totalsRowDxfId="24"/>
+    <tableColumn id="3" name="Prédécesseurs" dataDxfId="49" totalsRowDxfId="23"/>
+    <tableColumn id="4" name="Niveau de priorité" dataDxfId="48" totalsRowDxfId="22"/>
+    <tableColumn id="5" name="Niveau de difficulté" dataDxfId="47" totalsRowDxfId="21"/>
+    <tableColumn id="6" name="Temps requis (minutes)" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="20"/>
+    <tableColumn id="7" name="Prévision du Sprint où la tâche doit être terminée" dataDxfId="45" totalsRowDxfId="19"/>
+    <tableColumn id="8" name="Temps investis (minutes)" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="18"/>
+    <tableColumn id="9" name="% d'avancement au Sprint 1" dataDxfId="43" totalsRowDxfId="17"/>
+    <tableColumn id="10" name="% d'avancement au Sprint 2" dataDxfId="42" totalsRowDxfId="16"/>
+    <tableColumn id="11" name="% d'avancement au Sprint 3" dataDxfId="41" totalsRowDxfId="15"/>
+    <tableColumn id="12" name="% d'avancement au Sprint 4" dataDxfId="40" totalsRowDxfId="14"/>
+    <tableColumn id="13" name="Pourquoi le retard" dataDxfId="39" totalsRowDxfId="13"/>
+    <tableColumn id="14" name="Moyens envisagés pour solutionner le problème" dataDxfId="38" totalsRowDxfId="12"/>
+    <tableColumn id="15" name="Sprint 1" dataDxfId="37" totalsRowDxfId="11">
       <calculatedColumnFormula>IF(OR($H13="",J13=""),"Indef",IF(J13&gt;=1,"Terminé",IF($H13&lt;=P$12,"Retard",IF(J13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Sprint 2" dataDxfId="156" totalsRowDxfId="10">
+    <tableColumn id="16" name="Sprint 2" dataDxfId="36" totalsRowDxfId="10">
       <calculatedColumnFormula>IF(OR($H13="",K13=""),"Indef",IF(K13&gt;=1,"Terminé",IF($H13&lt;=Q$12,"Retard",IF(K13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Sprint 3" dataDxfId="155" totalsRowDxfId="9">
+    <tableColumn id="17" name="Sprint 3" dataDxfId="35" totalsRowDxfId="9">
       <calculatedColumnFormula>IF(OR($H13="",L13=""),"Indef",IF(L13&gt;=1,"Terminé",IF($H13&lt;=R$12,"Retard",IF(L13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Sprint 4" dataDxfId="154" totalsRowDxfId="8">
+    <tableColumn id="18" name="Sprint 4" dataDxfId="34" totalsRowDxfId="8">
       <calculatedColumnFormula>IF(OR($H13="",M13=""),"Indef",IF(M13&gt;=1,"Terminé",IF($H13&lt;=S$12,"Retard",IF(M13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Prev 00" dataDxfId="153" totalsRowDxfId="7">
+    <tableColumn id="25" name="Prev 00" dataDxfId="33" totalsRowDxfId="7">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Prev 01" dataDxfId="152" totalsRowDxfId="6">
+    <tableColumn id="26" name="Prev 01" dataDxfId="32" totalsRowDxfId="6">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Prev 02" dataDxfId="151" totalsRowDxfId="5">
+    <tableColumn id="27" name="Prev 02" dataDxfId="31" totalsRowDxfId="5">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Prev 03" dataDxfId="150" totalsRowDxfId="4">
+    <tableColumn id="28" name="Prev 03" dataDxfId="30" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 4",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Temps S1" dataDxfId="149" totalsRowDxfId="3">
+    <tableColumn id="21" name="Temps S1" dataDxfId="29" totalsRowDxfId="3">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Temps S2" dataDxfId="148" totalsRowDxfId="2">
+    <tableColumn id="23" name="Temps S2" dataDxfId="28" totalsRowDxfId="2">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Temps S3" dataDxfId="147" totalsRowDxfId="1">
+    <tableColumn id="22" name="Temps S3" dataDxfId="27" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Temps S4" dataDxfId="146" totalsRowDxfId="0">
+    <tableColumn id="24" name="Temps S4" dataDxfId="26" totalsRowDxfId="0">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 4",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5973,8 +4498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="11.25"/>
@@ -6000,22 +4525,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="19.5" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
       <c r="O1" s="40" t="s">
         <v>13</v>
       </c>
@@ -6031,7 +4556,7 @@
     </row>
     <row r="3" spans="1:34" ht="12" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="50" t="s">
         <v>72</v>
       </c>
       <c r="O3" s="28" t="s">
@@ -6040,37 +4565,37 @@
     </row>
     <row r="4" spans="1:34" ht="12" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="C4" s="45"/>
+      <c r="C4" s="51"/>
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:34" ht="12" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="C5" s="45"/>
+      <c r="C5" s="51"/>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:34" ht="12" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="C6" s="45"/>
+      <c r="C6" s="51"/>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:34" ht="12" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="C7" s="45"/>
+      <c r="C7" s="51"/>
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:34" ht="12" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="C8" s="45"/>
+      <c r="C8" s="51"/>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:34" ht="12" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="C9" s="45"/>
+      <c r="C9" s="51"/>
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:34" ht="12" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="C10" s="45"/>
+      <c r="C10" s="51"/>
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:34">
@@ -6274,7 +4799,7 @@
         <v>15</v>
       </c>
       <c r="I14" s="29">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J14" s="32">
         <v>0</v>
@@ -6328,7 +4853,7 @@
       </c>
       <c r="Y14" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z14" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
@@ -6370,7 +4895,7 @@
         <v>15</v>
       </c>
       <c r="I15" s="29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J15" s="32">
         <v>0</v>
@@ -6424,7 +4949,7 @@
       </c>
       <c r="Y15" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z15" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
@@ -6464,7 +4989,7 @@
         <v>15</v>
       </c>
       <c r="I16" s="29">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J16" s="32">
         <v>0</v>
@@ -6518,7 +5043,7 @@
       </c>
       <c r="Y16" s="18">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Z16" s="18">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
@@ -6560,7 +5085,7 @@
         <v>15</v>
       </c>
       <c r="I17" s="29">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J17" s="32">
         <v>0</v>
@@ -6614,7 +5139,7 @@
       </c>
       <c r="Y17" s="18">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Z17" s="18">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
@@ -6656,7 +5181,7 @@
         <v>15</v>
       </c>
       <c r="I18" s="29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J18" s="32">
         <v>0</v>
@@ -6710,7 +5235,7 @@
       </c>
       <c r="Y18" s="18">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z18" s="18">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
@@ -6748,37 +5273,41 @@
       <c r="G19" s="29">
         <v>30</v>
       </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="51">
-        <v>0</v>
-      </c>
-      <c r="K19" s="51">
+      <c r="H19" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="29">
+        <v>45</v>
+      </c>
+      <c r="J19" s="48">
+        <v>0</v>
+      </c>
+      <c r="K19" s="48">
         <v>0.8</v>
       </c>
-      <c r="L19" s="51">
-        <v>0</v>
-      </c>
-      <c r="M19" s="51">
+      <c r="L19" s="48">
+        <v>0</v>
+      </c>
+      <c r="M19" s="48">
         <v>0</v>
       </c>
       <c r="N19" s="34"/>
       <c r="O19" s="35"/>
       <c r="P19" s="8" t="str">
         <f>IF(OR($H19="",J19=""),"Indef",IF(J19&gt;=1,"Terminé",IF($H19&lt;=P$12,"Retard",IF(J19&gt;0,"Avancement","Sprint suivant"))))</f>
-        <v>Indef</v>
+        <v>Sprint suivant</v>
       </c>
       <c r="Q19" s="8" t="str">
         <f>IF(OR($H19="",K19=""),"Indef",IF(K19&gt;=1,"Terminé",IF($H19&lt;=Q$12,"Retard",IF(K19&gt;0,"Avancement","Sprint suivant"))))</f>
-        <v>Indef</v>
+        <v>Retard</v>
       </c>
       <c r="R19" s="8" t="str">
         <f>IF(OR($H19="",L19=""),"Indef",IF(L19&gt;=1,"Terminé",IF($H19&lt;=R$12,"Retard",IF(L19&gt;0,"Avancement","Sprint suivant"))))</f>
-        <v>Indef</v>
+        <v>Retard</v>
       </c>
       <c r="S19" s="8" t="str">
         <f>IF(OR($H19="",M19=""),"Indef",IF(M19&gt;=1,"Terminé",IF($H19&lt;=S$12,"Retard",IF(M19&gt;0,"Avancement","Sprint suivant"))))</f>
-        <v>Indef</v>
+        <v>Retard</v>
       </c>
       <c r="T19" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps requis (minutes)]],0)</f>
@@ -6786,7 +5315,7 @@
       </c>
       <c r="U19" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps requis (minutes)]],0)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="V19" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps requis (minutes)]],0)</f>
@@ -6802,7 +5331,7 @@
       </c>
       <c r="Y19" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="Z19" s="9">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
@@ -7030,7 +5559,7 @@
         <v>15</v>
       </c>
       <c r="I22" s="29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J22" s="32">
         <v>0</v>
@@ -7084,7 +5613,7 @@
       </c>
       <c r="Y22" s="18">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Z22" s="18">
         <f>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</f>
@@ -9487,26 +8016,26 @@
       <c r="H50" s="31"/>
       <c r="I50" s="38">
         <f>SUBTOTAL(109,[Temps investis (minutes)])</f>
-        <v>25</v>
-      </c>
-      <c r="J50" s="46"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="47"/>
-      <c r="M50" s="47"/>
+        <v>135</v>
+      </c>
+      <c r="J50" s="43"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="44"/>
       <c r="N50" s="34"/>
       <c r="O50" s="39"/>
-      <c r="P50" s="48"/>
-      <c r="Q50" s="48"/>
-      <c r="R50" s="48"/>
-      <c r="S50" s="48"/>
-      <c r="T50" s="48"/>
-      <c r="U50" s="48"/>
-      <c r="V50" s="48"/>
-      <c r="W50" s="48"/>
-      <c r="X50" s="48"/>
-      <c r="Y50" s="49"/>
-      <c r="Z50" s="48"/>
-      <c r="AA50" s="50"/>
+      <c r="P50" s="45"/>
+      <c r="Q50" s="45"/>
+      <c r="R50" s="45"/>
+      <c r="S50" s="45"/>
+      <c r="T50" s="45"/>
+      <c r="U50" s="45"/>
+      <c r="V50" s="45"/>
+      <c r="W50" s="45"/>
+      <c r="X50" s="45"/>
+      <c r="Y50" s="46"/>
+      <c r="Z50" s="45"/>
+      <c r="AA50" s="47"/>
     </row>
     <row r="51" spans="2:27">
       <c r="B51" s="27"/>
@@ -11394,19 +9923,19 @@
       </c>
       <c r="F192" s="3">
         <f>COUNTIF(Table1[Prévision du Sprint où la tâche doit être terminée],E192)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G192" s="26">
         <f>F192/$F$195</f>
-        <v>0.30555555555555558</v>
+        <v>0.32432432432432434</v>
       </c>
       <c r="H192" s="3">
         <f>SUM(Table1[Prev 01])</f>
-        <v>320</v>
+        <v>350</v>
       </c>
       <c r="I192" s="3">
         <f>SUM(Table1[Temps S2])</f>
-        <v>25</v>
+        <v>135</v>
       </c>
     </row>
     <row r="193" spans="5:9" hidden="1">
@@ -11419,7 +9948,7 @@
       </c>
       <c r="G193" s="26">
         <f>F193/$F$195</f>
-        <v>0.44444444444444442</v>
+        <v>0.43243243243243246</v>
       </c>
       <c r="H193" s="3">
         <f>SUM(Table1[Prev 02])</f>
@@ -11440,7 +9969,7 @@
       </c>
       <c r="G194" s="26">
         <f>F194/$F$195</f>
-        <v>0.25</v>
+        <v>0.24324324324324326</v>
       </c>
       <c r="H194" s="3">
         <f>SUM(Table1[Prev 03])</f>
@@ -11457,15 +9986,15 @@
       </c>
       <c r="F195" s="3">
         <f>SUM(F191:F194)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H195" s="3">
         <f>SUM(H191:H194)</f>
-        <v>1120</v>
+        <v>1150</v>
       </c>
       <c r="I195" s="3">
         <f>SUM(I191:I194)</f>
-        <v>25</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -11475,145 +10004,145 @@
     <mergeCell ref="C3:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:F26">
-    <cfRule type="cellIs" dxfId="106" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="51" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="52" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="53" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:M26">
-    <cfRule type="expression" dxfId="103" priority="42">
+    <cfRule type="expression" dxfId="90" priority="42">
       <formula>P13="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="43">
+    <cfRule type="expression" dxfId="89" priority="43">
       <formula>P13="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="44">
+    <cfRule type="expression" dxfId="88" priority="44">
       <formula>P13="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:F28">
-    <cfRule type="cellIs" dxfId="100" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="40" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="41" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:M28">
-    <cfRule type="expression" dxfId="97" priority="36">
+    <cfRule type="expression" dxfId="84" priority="36">
       <formula>P28="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="37">
+    <cfRule type="expression" dxfId="83" priority="37">
       <formula>P28="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="38">
+    <cfRule type="expression" dxfId="82" priority="38">
       <formula>P28="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:F43">
-    <cfRule type="cellIs" dxfId="94" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="34" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="35" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:M43">
-    <cfRule type="expression" dxfId="91" priority="30">
+    <cfRule type="expression" dxfId="78" priority="30">
       <formula>P29="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="31">
+    <cfRule type="expression" dxfId="77" priority="31">
       <formula>P29="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="32">
+    <cfRule type="expression" dxfId="76" priority="32">
       <formula>P29="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:F46">
-    <cfRule type="cellIs" dxfId="88" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="29" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:M46">
-    <cfRule type="expression" dxfId="85" priority="24">
+    <cfRule type="expression" dxfId="72" priority="24">
       <formula>P44="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="25">
+    <cfRule type="expression" dxfId="71" priority="25">
       <formula>P44="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="26">
+    <cfRule type="expression" dxfId="70" priority="26">
       <formula>P44="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:F27">
-    <cfRule type="cellIs" dxfId="82" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="22" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="23" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:M27">
-    <cfRule type="expression" dxfId="79" priority="18">
+    <cfRule type="expression" dxfId="66" priority="18">
       <formula>P27="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="19">
+    <cfRule type="expression" dxfId="65" priority="19">
       <formula>P27="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="20">
+    <cfRule type="expression" dxfId="64" priority="20">
       <formula>P27="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47:M47">
-    <cfRule type="expression" dxfId="76" priority="15">
+    <cfRule type="expression" dxfId="63" priority="15">
       <formula>P47="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="16">
+    <cfRule type="expression" dxfId="62" priority="16">
       <formula>P47="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="17">
+    <cfRule type="expression" dxfId="61" priority="17">
       <formula>P47="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:M48">
-    <cfRule type="expression" dxfId="73" priority="12">
+    <cfRule type="expression" dxfId="60" priority="12">
       <formula>P48="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="13">
+    <cfRule type="expression" dxfId="59" priority="13">
       <formula>P48="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="14">
+    <cfRule type="expression" dxfId="58" priority="14">
       <formula>P48="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:M49">
-    <cfRule type="expression" dxfId="70" priority="9">
+    <cfRule type="expression" dxfId="57" priority="9">
       <formula>P49="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="10">
+    <cfRule type="expression" dxfId="56" priority="10">
       <formula>P49="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="11">
+    <cfRule type="expression" dxfId="55" priority="11">
       <formula>P49="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added room drawing, upped the resolution to 1024x768.
Functionality for custom resolutions or room sizes not present as intended.

Signed-off-by: Eltee <rjlb.lt@gmail.com>
</commit_message>
<xml_diff>
--- a/Docs/B65_S1_Planification_Renaud_Bigras.xlsx
+++ b/Docs/B65_S1_Planification_Renaud_Bigras.xlsx
@@ -380,6 +380,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="K20" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mr. Eltee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+La classe Room semble fonctionné comme prévu.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C21" authorId="0">
       <text>
         <r>
@@ -401,6 +425,30 @@
           </rPr>
           <t xml:space="preserve">
 Coder un algo d'affichage de la matrice de la salle avec le tileset inclus.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K21" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mr. Eltee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+La méthode draw appel la nouvelle méthode draw du tileset, qui recoit la tuile et la passe dans une switch pour decider quoi dessiner.</t>
         </r>
       </text>
     </comment>
@@ -1892,7 +1940,1405 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="94">
+  <dxfs count="211">
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2426,6 +3872,1404 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF255B01"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAFEC2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF255B01"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF255B01"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF255B01"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF255B01"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF5B0101"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEDEDE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B0101"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B0101"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B0101"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B0101"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF01125B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD2DAFE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF05015B"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF05015B"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF05015B"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF05015B"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA4A400"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFA40000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3014,705 +5858,6 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF255B01"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAFEC2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF255B01"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF255B01"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF255B01"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF255B01"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B0101"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEDEDE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B0101"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B0101"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B0101"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B0101"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF01125B"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2DAFE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF05015B"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF05015B"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF05015B"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF05015B"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA4A400"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA40000"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3851,7 +5996,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3996,11 +6141,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="96957952"/>
-        <c:axId val="96959488"/>
+        <c:axId val="82872192"/>
+        <c:axId val="82873728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96957952"/>
+        <c:axId val="82872192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4016,14 +6161,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96959488"/>
+        <c:crossAx val="82873728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96959488"/>
+        <c:axId val="82873728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4059,7 +6204,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96957952"/>
+        <c:crossAx val="82872192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4082,7 +6227,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4154,56 +6299,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:AA50" totalsRowCount="1" headerRowDxfId="54" dataDxfId="53" totalsRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:AA50" totalsRowCount="1" headerRowDxfId="210" dataDxfId="209" totalsRowDxfId="208">
   <tableColumns count="26">
-    <tableColumn id="1" name="Numéro de tâche" dataDxfId="51" totalsRowDxfId="25"/>
-    <tableColumn id="2" name="Description générale de la tâche" totalsRowFunction="count" dataDxfId="50" totalsRowDxfId="24"/>
-    <tableColumn id="3" name="Prédécesseurs" dataDxfId="49" totalsRowDxfId="23"/>
-    <tableColumn id="4" name="Niveau de priorité" dataDxfId="48" totalsRowDxfId="22"/>
-    <tableColumn id="5" name="Niveau de difficulté" dataDxfId="47" totalsRowDxfId="21"/>
-    <tableColumn id="6" name="Temps requis (minutes)" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="20"/>
-    <tableColumn id="7" name="Prévision du Sprint où la tâche doit être terminée" dataDxfId="45" totalsRowDxfId="19"/>
-    <tableColumn id="8" name="Temps investis (minutes)" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="18"/>
-    <tableColumn id="9" name="% d'avancement au Sprint 1" dataDxfId="43" totalsRowDxfId="17"/>
-    <tableColumn id="10" name="% d'avancement au Sprint 2" dataDxfId="42" totalsRowDxfId="16"/>
-    <tableColumn id="11" name="% d'avancement au Sprint 3" dataDxfId="41" totalsRowDxfId="15"/>
-    <tableColumn id="12" name="% d'avancement au Sprint 4" dataDxfId="40" totalsRowDxfId="14"/>
-    <tableColumn id="13" name="Pourquoi le retard" dataDxfId="39" totalsRowDxfId="13"/>
-    <tableColumn id="14" name="Moyens envisagés pour solutionner le problème" dataDxfId="38" totalsRowDxfId="12"/>
-    <tableColumn id="15" name="Sprint 1" dataDxfId="37" totalsRowDxfId="11">
+    <tableColumn id="1" name="Numéro de tâche" dataDxfId="207" totalsRowDxfId="103"/>
+    <tableColumn id="2" name="Description générale de la tâche" totalsRowFunction="count" dataDxfId="206" totalsRowDxfId="102"/>
+    <tableColumn id="3" name="Prédécesseurs" dataDxfId="205" totalsRowDxfId="101"/>
+    <tableColumn id="4" name="Niveau de priorité" dataDxfId="204" totalsRowDxfId="100"/>
+    <tableColumn id="5" name="Niveau de difficulté" dataDxfId="203" totalsRowDxfId="99"/>
+    <tableColumn id="6" name="Temps requis (minutes)" totalsRowFunction="sum" dataDxfId="202" totalsRowDxfId="98"/>
+    <tableColumn id="7" name="Prévision du Sprint où la tâche doit être terminée" dataDxfId="201" totalsRowDxfId="97"/>
+    <tableColumn id="8" name="Temps investis (minutes)" totalsRowFunction="sum" dataDxfId="200" totalsRowDxfId="96"/>
+    <tableColumn id="9" name="% d'avancement au Sprint 1" dataDxfId="199" totalsRowDxfId="95"/>
+    <tableColumn id="10" name="% d'avancement au Sprint 2" dataDxfId="198" totalsRowDxfId="94"/>
+    <tableColumn id="11" name="% d'avancement au Sprint 3" dataDxfId="197" totalsRowDxfId="93"/>
+    <tableColumn id="12" name="% d'avancement au Sprint 4" dataDxfId="196" totalsRowDxfId="92"/>
+    <tableColumn id="13" name="Pourquoi le retard" dataDxfId="195" totalsRowDxfId="91"/>
+    <tableColumn id="14" name="Moyens envisagés pour solutionner le problème" dataDxfId="194" totalsRowDxfId="90"/>
+    <tableColumn id="15" name="Sprint 1" dataDxfId="193" totalsRowDxfId="89">
       <calculatedColumnFormula>IF(OR($H13="",J13=""),"Indef",IF(J13&gt;=1,"Terminé",IF($H13&lt;=P$12,"Retard",IF(J13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Sprint 2" dataDxfId="36" totalsRowDxfId="10">
+    <tableColumn id="16" name="Sprint 2" dataDxfId="192" totalsRowDxfId="88">
       <calculatedColumnFormula>IF(OR($H13="",K13=""),"Indef",IF(K13&gt;=1,"Terminé",IF($H13&lt;=Q$12,"Retard",IF(K13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Sprint 3" dataDxfId="35" totalsRowDxfId="9">
+    <tableColumn id="17" name="Sprint 3" dataDxfId="191" totalsRowDxfId="87">
       <calculatedColumnFormula>IF(OR($H13="",L13=""),"Indef",IF(L13&gt;=1,"Terminé",IF($H13&lt;=R$12,"Retard",IF(L13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Sprint 4" dataDxfId="34" totalsRowDxfId="8">
+    <tableColumn id="18" name="Sprint 4" dataDxfId="190" totalsRowDxfId="86">
       <calculatedColumnFormula>IF(OR($H13="",M13=""),"Indef",IF(M13&gt;=1,"Terminé",IF($H13&lt;=S$12,"Retard",IF(M13&gt;0,"Avancement","Sprint suivant"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Prev 00" dataDxfId="33" totalsRowDxfId="7">
+    <tableColumn id="25" name="Prev 00" dataDxfId="189" totalsRowDxfId="85">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Prev 01" dataDxfId="32" totalsRowDxfId="6">
+    <tableColumn id="26" name="Prev 01" dataDxfId="188" totalsRowDxfId="84">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Prev 02" dataDxfId="31" totalsRowDxfId="5">
+    <tableColumn id="27" name="Prev 02" dataDxfId="187" totalsRowDxfId="83">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Prev 03" dataDxfId="30" totalsRowDxfId="4">
+    <tableColumn id="28" name="Prev 03" dataDxfId="186" totalsRowDxfId="82">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 4",Table1[[#This Row],[Temps requis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Temps S1" dataDxfId="29" totalsRowDxfId="3">
+    <tableColumn id="21" name="Temps S1" dataDxfId="185" totalsRowDxfId="81">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 1",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="Temps S2" dataDxfId="28" totalsRowDxfId="2">
+    <tableColumn id="23" name="Temps S2" dataDxfId="184" totalsRowDxfId="80">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 2",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Temps S3" dataDxfId="27" totalsRowDxfId="1">
+    <tableColumn id="22" name="Temps S3" dataDxfId="183" totalsRowDxfId="79">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 3",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="Temps S4" dataDxfId="26" totalsRowDxfId="0">
+    <tableColumn id="24" name="Temps S4" dataDxfId="182" totalsRowDxfId="78">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Prévision du Sprint où la tâche doit être terminée]]="Sprint 4",Table1[[#This Row],[Temps investis (minutes)]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4498,8 +6643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="11.25"/>
@@ -5377,7 +7522,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L20" s="33">
         <v>0</v>
@@ -5472,7 +7617,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="33">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="L21" s="33">
         <v>0</v>
@@ -10004,150 +12149,150 @@
     <mergeCell ref="C3:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:F26">
-    <cfRule type="cellIs" dxfId="93" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="54" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="55" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="56" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:M26">
-    <cfRule type="expression" dxfId="90" priority="42">
+    <cfRule type="expression" dxfId="74" priority="45">
       <formula>P13="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="43">
+    <cfRule type="expression" dxfId="73" priority="46">
       <formula>P13="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="44">
+    <cfRule type="expression" dxfId="72" priority="47">
       <formula>P13="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:F28">
-    <cfRule type="cellIs" dxfId="87" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="43" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="44" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:M28">
-    <cfRule type="expression" dxfId="84" priority="36">
+    <cfRule type="expression" dxfId="68" priority="39">
       <formula>P28="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="37">
+    <cfRule type="expression" dxfId="67" priority="40">
       <formula>P28="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="38">
+    <cfRule type="expression" dxfId="66" priority="41">
       <formula>P28="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:F43">
-    <cfRule type="cellIs" dxfId="81" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="37" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="38" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:M43">
-    <cfRule type="expression" dxfId="78" priority="30">
+    <cfRule type="expression" dxfId="62" priority="33">
       <formula>P29="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="31">
+    <cfRule type="expression" dxfId="61" priority="34">
       <formula>P29="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="32">
+    <cfRule type="expression" dxfId="60" priority="35">
       <formula>P29="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:F46">
-    <cfRule type="cellIs" dxfId="75" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="31" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="32" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:M46">
-    <cfRule type="expression" dxfId="72" priority="24">
+    <cfRule type="expression" dxfId="56" priority="27">
       <formula>P44="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="25">
+    <cfRule type="expression" dxfId="55" priority="28">
       <formula>P44="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="26">
+    <cfRule type="expression" dxfId="54" priority="29">
       <formula>P44="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:F27">
-    <cfRule type="cellIs" dxfId="69" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="25" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="26" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:M27">
-    <cfRule type="expression" dxfId="66" priority="18">
+    <cfRule type="expression" dxfId="50" priority="21">
       <formula>P27="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="19">
+    <cfRule type="expression" dxfId="49" priority="22">
       <formula>P27="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="20">
+    <cfRule type="expression" dxfId="48" priority="23">
       <formula>P27="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47:M47">
-    <cfRule type="expression" dxfId="63" priority="15">
+    <cfRule type="expression" dxfId="47" priority="18">
       <formula>P47="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="16">
+    <cfRule type="expression" dxfId="46" priority="19">
       <formula>P47="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="17">
+    <cfRule type="expression" dxfId="45" priority="20">
       <formula>P47="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:M48">
-    <cfRule type="expression" dxfId="60" priority="12">
+    <cfRule type="expression" dxfId="44" priority="15">
       <formula>P48="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="13">
+    <cfRule type="expression" dxfId="43" priority="16">
       <formula>P48="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="14">
+    <cfRule type="expression" dxfId="42" priority="17">
       <formula>P48="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:M49">
-    <cfRule type="expression" dxfId="57" priority="9">
+    <cfRule type="expression" dxfId="41" priority="12">
       <formula>P49="Avancement"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="10">
+    <cfRule type="expression" dxfId="40" priority="13">
       <formula>P49="Retard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="11">
+    <cfRule type="expression" dxfId="39" priority="14">
       <formula>P49="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -10157,7 +12302,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -10167,7 +12312,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -10177,6 +12322,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10186,8 +12361,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
+  <conditionalFormatting sqref="K19">
     <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -10196,33 +12381,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
+  <conditionalFormatting sqref="K21">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>